<commit_message>
Performance analysis of DCB in spatially distributed WLANs
Results from paper S. Barrachina-Muñoz, F. Wilhelmi, and B. Bellalta. Performance of Dynamic Channel Bonding in Spatially Distributed High Density WLANs. arXiv preprint arXiv:1801.00594, 2018.
</commit_message>
<xml_diff>
--- a/results/march14analysis/results.xlsx
+++ b/results/march14analysis/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Spatial</t>
   </si>
@@ -70,12 +70,6 @@
   </si>
   <si>
     <t>Some overlapping (500 m)</t>
-  </si>
-  <si>
-    <t>primary only</t>
-  </si>
-  <si>
-    <t>potencia tx entre num canals</t>
   </si>
   <si>
     <t>Proportional Fairness</t>
@@ -345,73 +339,73 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -710,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="E24" sqref="A17:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -729,71 +723,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="25" t="s">
-        <v>20</v>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21" t="s">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="25"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="4">
         <v>6</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="4">
         <v>6</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="19">
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="10">
         <v>228.81</v>
       </c>
       <c r="J3" s="2">
@@ -801,21 +795,21 @@
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="4">
         <v>15</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="4">
         <v>11</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="17">
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="8">
         <v>392.84980000000002</v>
       </c>
       <c r="J4" s="1">
@@ -823,21 +817,21 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="4">
         <v>77</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="4">
         <v>72</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="11">
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="5">
         <v>302.39</v>
       </c>
       <c r="J5" s="1">
@@ -845,204 +839,189 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="25"/>
+      <c r="B6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="6">
         <v>77</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="6">
         <v>77</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="18">
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="9">
         <v>334.78410000000002</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>16</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>16</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="23">
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="13">
         <v>606.75879999999995</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="4">
         <v>16</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="4">
         <v>16</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="24">
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="14">
         <v>606.75879999999995</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="24"/>
+      <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="4">
         <v>180</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="4">
         <v>133</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="11">
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="5">
         <v>371.04399999999998</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" thickBot="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13" t="s">
+      <c r="A10" s="25"/>
+      <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="6">
         <v>180</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="6">
         <v>180</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="16">
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="7">
         <v>457.17</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="3">
         <v>10</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="23">
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="13">
         <v>441.34</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="24"/>
+      <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="4">
         <v>16</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="4">
         <v>11</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="24">
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="14">
         <v>443.03059999999999</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="24"/>
+      <c r="B13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="4">
         <v>93</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="4">
         <v>88</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="11">
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="5">
         <v>302.55</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" thickBot="1">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="25"/>
+      <c r="B14" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="6">
         <v>93</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="6">
         <v>93</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="18">
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="9">
         <v>335.39600000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="C21" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E3:H6"/>
-    <mergeCell ref="E7:H10"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="E11:H14"/>
     <mergeCell ref="A3:A6"/>
@@ -1050,6 +1029,11 @@
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="E1:I1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E3:H6"/>
+    <mergeCell ref="E7:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>